<commit_message>
latest changes - 16-03-2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
+++ b/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HL\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD745D0B-DBA9-4941-930A-6BF0AB12B212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09E8FF8-D5CC-45E4-87CD-5D0B28D19378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="StartDateFilterOptions" sheetId="8" r:id="rId2"/>
     <sheet name="KPIMetrics" sheetId="9" r:id="rId3"/>
-    <sheet name="Activity" sheetId="4" r:id="rId4"/>
+    <sheet name="ActivityColumns" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,41 +28,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Users</t>
   </si>
   <si>
-    <t>ActivityCompany</t>
-  </si>
-  <si>
-    <t>ActivityType</t>
-  </si>
-  <si>
-    <t>ActivitySubject</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Internal Notes</t>
-  </si>
-  <si>
-    <t>Lookup Company</t>
-  </si>
-  <si>
-    <t>Meeting</t>
-  </si>
-  <si>
-    <t>TestDescription</t>
-  </si>
-  <si>
-    <t>TestInternalNotes</t>
-  </si>
-  <si>
-    <t>Test Subject</t>
-  </si>
-  <si>
     <t>Last 7 Days</t>
   </si>
   <si>
@@ -118,6 +91,39 @@
   </si>
   <si>
     <t>Missing Notes</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>Event/Task Type</t>
+  </si>
+  <si>
+    <t>HL Contact</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Meeting/Call Notes</t>
+  </si>
+  <si>
+    <t>External Contact</t>
   </si>
 </sst>
 </file>
@@ -164,9 +170,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +469,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -489,57 +493,57 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -552,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F867BB15-8B6C-4F1B-B262-3A41B97B60E4}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,37 +567,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -604,50 +608,77 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
company coverage dashboard script changes, wedriver update - 03 April 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
+++ b/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09E8FF8-D5CC-45E4-87CD-5D0B28D19378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12233264-D9CC-42D4-88E3-884571C196D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
-    <sheet name="StartDateFilterOptions" sheetId="8" r:id="rId2"/>
-    <sheet name="KPIMetrics" sheetId="9" r:id="rId3"/>
-    <sheet name="ActivityColumns" sheetId="4" r:id="rId4"/>
+    <sheet name="Company" sheetId="10" r:id="rId2"/>
+    <sheet name="StartDateFilterOptions" sheetId="8" r:id="rId3"/>
+    <sheet name="KPIMetrics" sheetId="9" r:id="rId4"/>
+    <sheet name="ActivityColumns" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Users</t>
   </si>
@@ -69,61 +70,67 @@
     <t>StartDateFilterOptions</t>
   </si>
   <si>
+    <t>KPIMetrics</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Meetings</t>
+  </si>
+  <si>
+    <t>Calls</t>
+  </si>
+  <si>
+    <t>Emails/Tasks</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Missing Notes</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>Event/Task Type</t>
+  </si>
+  <si>
+    <t>HL Contact</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Meeting/Call Notes</t>
+  </si>
+  <si>
+    <t>External Contact</t>
+  </si>
+  <si>
     <t>William Peluchiwski</t>
   </si>
   <si>
-    <t>KPIMetrics</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Meetings</t>
-  </si>
-  <si>
-    <t>Calls</t>
-  </si>
-  <si>
-    <t>Emails/Tasks</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>Missing Notes</t>
-  </si>
-  <si>
-    <t>Columns</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Tier</t>
-  </si>
-  <si>
-    <t>Event/Task Type</t>
-  </si>
-  <si>
-    <t>HL Contact</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Meeting/Call Notes</t>
-  </si>
-  <si>
-    <t>External Contact</t>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>International Wire Group, Inc.</t>
   </si>
 </sst>
 </file>
@@ -167,10 +174,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +460,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,7 +475,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -479,6 +485,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7972DAA3-2502-4122-BD46-655C1E9DC13D}">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -552,7 +584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F867BB15-8B6C-4F1B-B262-3A41B97B60E4}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -567,37 +599,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -606,11 +638,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -618,63 +650,63 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Coverage Company Dashboard script changes - 04 Apr
</commit_message>
<xml_diff>
--- a/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
+++ b/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12233264-D9CC-42D4-88E3-884571C196D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F148CD-37EE-47C7-98E7-16765CAAB407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="StartDateFilterOptions" sheetId="8" r:id="rId3"/>
     <sheet name="KPIMetrics" sheetId="9" r:id="rId4"/>
     <sheet name="ActivityColumns" sheetId="4" r:id="rId5"/>
+    <sheet name="Activity" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Users</t>
   </si>
@@ -131,6 +132,33 @@
   </si>
   <si>
     <t>International Wire Group, Inc.</t>
+  </si>
+  <si>
+    <t>IndustryGroup</t>
+  </si>
+  <si>
+    <t>ProductType</t>
+  </si>
+  <si>
+    <t>MeetingNotes</t>
+  </si>
+  <si>
+    <t>ExtAttendee</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Test Conf 01</t>
+  </si>
+  <si>
+    <t>BUS - Business Services</t>
+  </si>
+  <si>
+    <t>Activist Advisory</t>
+  </si>
+  <si>
+    <t>Test External</t>
   </si>
 </sst>
 </file>
@@ -174,9 +202,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,4 +744,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rework on Company Coverage Dashboard script TMTT00022150 - 31 July 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
+++ b/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F148CD-37EE-47C7-98E7-16765CAAB407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356EB8D0-71B3-444F-A372-66080DBB560B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Users</t>
   </si>
@@ -98,67 +98,73 @@
     <t>#</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Event/Task Type</t>
+  </si>
+  <si>
+    <t>HL Contact</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Meeting/Call Notes</t>
+  </si>
+  <si>
+    <t>External Contact</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>International Wire Group, Inc.</t>
+  </si>
+  <si>
+    <t>IndustryGroup</t>
+  </si>
+  <si>
+    <t>ProductType</t>
+  </si>
+  <si>
+    <t>MeetingNotes</t>
+  </si>
+  <si>
+    <t>ExtAttendee</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Test Conf 01</t>
+  </si>
+  <si>
+    <t>BUS - Business Services</t>
+  </si>
+  <si>
+    <t>Activist Advisory</t>
+  </si>
+  <si>
+    <t>Test External</t>
+  </si>
+  <si>
+    <t>James Craven</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Tier</t>
-  </si>
-  <si>
-    <t>Event/Task Type</t>
-  </si>
-  <si>
-    <t>HL Contact</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Meeting/Call Notes</t>
-  </si>
-  <si>
-    <t>External Contact</t>
-  </si>
-  <si>
-    <t>William Peluchiwski</t>
-  </si>
-  <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>International Wire Group, Inc.</t>
-  </si>
-  <si>
-    <t>IndustryGroup</t>
-  </si>
-  <si>
-    <t>ProductType</t>
-  </si>
-  <si>
-    <t>MeetingNotes</t>
-  </si>
-  <si>
-    <t>ExtAttendee</t>
-  </si>
-  <si>
-    <t>Meeting</t>
-  </si>
-  <si>
-    <t>Test Conf 01</t>
-  </si>
-  <si>
-    <t>BUS - Business Services</t>
-  </si>
-  <si>
-    <t>Activist Advisory</t>
-  </si>
-  <si>
-    <t>Test External</t>
   </si>
 </sst>
 </file>
@@ -491,7 +497,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,7 +512,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -527,12 +533,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -671,10 +677,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,52 +698,57 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -750,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -766,48 +777,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Changes - TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality- 1st Aug 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
+++ b/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356EB8D0-71B3-444F-A372-66080DBB560B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C81073-7B93-4DD2-8A0E-687B9C15617C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>CompanyName</t>
   </si>
   <si>
-    <t>International Wire Group, Inc.</t>
-  </si>
-  <si>
     <t>IndustryGroup</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>StandardTestCompany</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -679,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -698,22 +698,22 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -723,7 +723,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -783,42 +783,42 @@
         <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
         <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality - 29 April 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
+++ b/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C81073-7B93-4DD2-8A0E-687B9C15617C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484AC289-2492-4808-8981-5C12EE89D7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -146,25 +146,25 @@
     <t>Test External</t>
   </si>
   <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>StandardTestCompany</t>
+  </si>
+  <si>
     <t>James Craven</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>..</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Tier</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>StandardTestCompany</t>
   </si>
 </sst>
 </file>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +512,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -538,7 +538,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -698,22 +698,22 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -723,7 +723,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality - 1 May 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
+++ b/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484AC289-2492-4808-8981-5C12EE89D7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E93C2D6-751E-4EEA-A961-926FABE7C502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="528" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -164,7 +164,7 @@
     <t>StandardTestCompany</t>
   </si>
   <si>
-    <t>James Craven</t>
+    <t>Sahil Mittal</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Company Coverage dashboard - 1st May 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
+++ b/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E93C2D6-751E-4EEA-A961-926FABE7C502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8191BB-9956-4744-9743-4AD3E4BFEC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="528" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="528" windowWidth="21384" windowHeight="10548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Users</t>
   </si>
@@ -146,12 +146,6 @@
     <t>Test External</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>..</t>
-  </si>
-  <si>
     <t>Company Name</t>
   </si>
   <si>
@@ -161,10 +155,22 @@
     <t>Date</t>
   </si>
   <si>
-    <t>StandardTestCompany</t>
-  </si>
-  <si>
-    <t>Sahil Mittal</t>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Companies Discussed</t>
+  </si>
+  <si>
+    <t>External Contact Company</t>
+  </si>
+  <si>
+    <t>CapProviderTestCompany</t>
+  </si>
+  <si>
+    <t>Indrajeet Singh</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +518,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -526,7 +532,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +544,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -677,10 +683,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,22 +704,22 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -723,7 +729,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -743,12 +749,22 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Company Coverage Dashboard Final - 1st May 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
+++ b/TestData/TMTT0022150_VerificationOfCoverageCompanyDashboardNewUIAndFunctionality.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8191BB-9956-4744-9743-4AD3E4BFEC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D67402-1842-4D98-A5BF-907FC6F240B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="528" windowWidth="21384" windowHeight="10548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,7 +170,7 @@
     <t>CapProviderTestCompany</t>
   </si>
   <si>
-    <t>Indrajeet Singh</t>
+    <t>James Craven</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>